<commit_message>
level up exp config
</commit_message>
<xml_diff>
--- a/plan/excel/hero_英雄表.xlsx
+++ b/plan/excel/hero_英雄表.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HeroProto" sheetId="4" r:id="rId1"/>
+    <sheet name="LevelupExp" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HeroProto!$A$1:$J$4</definedName>
@@ -74,31 +75,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">1 客户端专用
-2 服务器专用
-3 通用
-0 策划维护用
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
   <si>
     <t>英雄ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -345,6 +327,14 @@
   <si>
     <t>model</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>经验</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -738,9 +728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1687,4 +1677,252 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>26000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hero levelup & hero refine
</commit_message>
<xml_diff>
--- a/plan/excel/hero_英雄表.xlsx
+++ b/plan/excel/hero_英雄表.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="HeroProto" sheetId="4" r:id="rId1"/>
-    <sheet name="LevelupExp" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HeroProto!$A$1:$J$4</definedName>
@@ -80,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="49">
   <si>
     <t>英雄ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -329,12 +328,36 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>经验</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>exp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>晋级材料</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>jl</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4113_1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>4113_2</t>
+  </si>
+  <si>
+    <t>4113_3</t>
+  </si>
+  <si>
+    <t>4113_4</t>
+  </si>
+  <si>
+    <t>4113_5</t>
+  </si>
+  <si>
+    <t>needs#id_cnt</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -726,11 +749,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -741,9 +764,10 @@
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="7.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.125" customWidth="1"/>
+    <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -774,8 +798,11 @@
       <c r="J1" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -806,8 +833,11 @@
       <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -838,8 +868,11 @@
       <c r="J3" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -870,8 +903,11 @@
       <c r="J4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>5001</v>
       </c>
@@ -902,8 +938,11 @@
       <c r="J5" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5001</v>
       </c>
@@ -934,8 +973,11 @@
       <c r="J6" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5001</v>
       </c>
@@ -966,8 +1008,11 @@
       <c r="J7" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5001</v>
       </c>
@@ -998,8 +1043,11 @@
       <c r="J8" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K8" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>5001</v>
       </c>
@@ -1030,8 +1078,11 @@
       <c r="J9" s="4">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>5002</v>
       </c>
@@ -1062,8 +1113,11 @@
       <c r="J10" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>5002</v>
       </c>
@@ -1094,8 +1148,11 @@
       <c r="J11" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>5002</v>
       </c>
@@ -1126,8 +1183,11 @@
       <c r="J12" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K12" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>5002</v>
       </c>
@@ -1158,8 +1218,11 @@
       <c r="J13" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K13" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>5002</v>
       </c>
@@ -1190,8 +1253,11 @@
       <c r="J14" s="4">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K14" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>5003</v>
       </c>
@@ -1222,8 +1288,11 @@
       <c r="J15" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>5003</v>
       </c>
@@ -1254,8 +1323,11 @@
       <c r="J16" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K16" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>5003</v>
       </c>
@@ -1286,8 +1358,11 @@
       <c r="J17" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>5003</v>
       </c>
@@ -1318,8 +1393,11 @@
       <c r="J18" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K18" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>5003</v>
       </c>
@@ -1350,8 +1428,11 @@
       <c r="J19" s="4">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K19" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>5004</v>
       </c>
@@ -1382,8 +1463,11 @@
       <c r="J20" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K20" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>5004</v>
       </c>
@@ -1414,8 +1498,11 @@
       <c r="J21" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K21" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>5004</v>
       </c>
@@ -1446,8 +1533,11 @@
       <c r="J22" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K22" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>5004</v>
       </c>
@@ -1478,8 +1568,11 @@
       <c r="J23" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K23" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>5004</v>
       </c>
@@ -1510,8 +1603,11 @@
       <c r="J24" s="4">
         <v>60</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K24" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>5005</v>
       </c>
@@ -1542,8 +1638,11 @@
       <c r="J25" s="4">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K25" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>5005</v>
       </c>
@@ -1574,8 +1673,11 @@
       <c r="J26" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K26" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>5005</v>
       </c>
@@ -1606,8 +1708,11 @@
       <c r="J27" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K27" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>5005</v>
       </c>
@@ -1638,8 +1743,11 @@
       <c r="J28" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K28" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>5005</v>
       </c>
@@ -1669,6 +1777,9 @@
       </c>
       <c r="J29" s="4">
         <v>60</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1677,252 +1788,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16">
-        <v>12</v>
-      </c>
-      <c r="B16">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17">
-        <v>13</v>
-      </c>
-      <c r="B17">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18">
-        <v>14</v>
-      </c>
-      <c r="B18">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19">
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20">
-        <v>16</v>
-      </c>
-      <c r="B20">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22">
-        <v>18</v>
-      </c>
-      <c r="B22">
-        <v>19000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23">
-        <v>19</v>
-      </c>
-      <c r="B23">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24">
-        <v>20</v>
-      </c>
-      <c r="B24">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25">
-        <v>21</v>
-      </c>
-      <c r="B25">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>22</v>
-      </c>
-      <c r="B26">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>23</v>
-      </c>
-      <c r="B27">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29">
-        <v>25</v>
-      </c>
-      <c r="B29">
-        <v>26000</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
hero skill & levelup event
</commit_message>
<xml_diff>
--- a/plan/excel/hero_英雄表.xlsx
+++ b/plan/excel/hero_英雄表.xlsx
@@ -10,7 +10,7 @@
     <sheet name="HeroProto" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HeroProto!$A$1:$J$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HeroProto!$A$1:$L$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -22,7 +22,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="53">
   <si>
     <t>英雄ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -357,6 +357,22 @@
   </si>
   <si>
     <t>needs#id_cnt</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能一</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能二</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill_2</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -749,11 +765,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -762,12 +778,13 @@
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" customWidth="1"/>
-    <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.125" customWidth="1"/>
+    <col min="13" max="13" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -784,25 +801,31 @@
         <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -819,25 +842,31 @@
         <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -854,25 +883,31 @@
         <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -888,11 +923,11 @@
       <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>2</v>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>2</v>
@@ -903,11 +938,17 @@
       <c r="J4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>5001</v>
       </c>
@@ -923,26 +964,32 @@
       <c r="E5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
+        <v>1002</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1003</v>
+      </c>
+      <c r="H5">
         <v>100</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>80</v>
       </c>
-      <c r="H5" s="4">
+      <c r="J5" s="4">
         <v>1000</v>
       </c>
-      <c r="I5" s="4">
-        <v>5</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="K5" s="4">
+        <v>5</v>
+      </c>
+      <c r="L5" s="4">
         <v>40</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5001</v>
       </c>
@@ -958,26 +1005,28 @@
       <c r="E6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6">
         <v>120</v>
       </c>
-      <c r="G6" s="2">
+      <c r="I6" s="2">
         <v>90</v>
       </c>
-      <c r="H6" s="4">
+      <c r="J6" s="4">
         <v>1100</v>
       </c>
-      <c r="I6" s="4">
-        <v>5</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
+        <v>5</v>
+      </c>
+      <c r="L6" s="4">
         <v>45</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5001</v>
       </c>
@@ -993,26 +1042,28 @@
       <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7">
         <v>140</v>
       </c>
-      <c r="G7" s="2">
+      <c r="I7" s="2">
         <v>100</v>
       </c>
-      <c r="H7" s="4">
+      <c r="J7" s="4">
         <v>1200</v>
       </c>
-      <c r="I7" s="4">
-        <v>5</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
+        <v>5</v>
+      </c>
+      <c r="L7" s="4">
         <v>50</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5001</v>
       </c>
@@ -1028,26 +1079,28 @@
       <c r="E8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8">
         <v>160</v>
       </c>
-      <c r="G8" s="2">
+      <c r="I8" s="2">
         <v>110</v>
       </c>
-      <c r="H8" s="4">
+      <c r="J8" s="4">
         <v>1300</v>
       </c>
-      <c r="I8" s="4">
-        <v>5</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
+        <v>5</v>
+      </c>
+      <c r="L8" s="4">
         <v>55</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>5001</v>
       </c>
@@ -1063,26 +1116,28 @@
       <c r="E9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9">
         <v>180</v>
       </c>
-      <c r="G9" s="2">
+      <c r="I9" s="2">
         <v>120</v>
       </c>
-      <c r="H9" s="4">
+      <c r="J9" s="4">
         <v>1400</v>
       </c>
-      <c r="I9" s="4">
-        <v>5</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4">
         <v>60</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>5002</v>
       </c>
@@ -1098,26 +1153,32 @@
       <c r="E10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
+        <v>1002</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1003</v>
+      </c>
+      <c r="H10">
         <v>100</v>
       </c>
-      <c r="G10" s="2">
+      <c r="I10" s="2">
         <v>80</v>
       </c>
-      <c r="H10" s="4">
+      <c r="J10" s="4">
         <v>1000</v>
       </c>
-      <c r="I10" s="4">
-        <v>5</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
+        <v>5</v>
+      </c>
+      <c r="L10" s="4">
         <v>40</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>5002</v>
       </c>
@@ -1133,26 +1194,28 @@
       <c r="E11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11">
         <v>120</v>
       </c>
-      <c r="G11" s="2">
+      <c r="I11" s="2">
         <v>90</v>
       </c>
-      <c r="H11" s="4">
+      <c r="J11" s="4">
         <v>1100</v>
       </c>
-      <c r="I11" s="4">
-        <v>5</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
+        <v>5</v>
+      </c>
+      <c r="L11" s="4">
         <v>45</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>5002</v>
       </c>
@@ -1168,26 +1231,28 @@
       <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12">
         <v>140</v>
       </c>
-      <c r="G12" s="2">
+      <c r="I12" s="2">
         <v>100</v>
       </c>
-      <c r="H12" s="4">
+      <c r="J12" s="4">
         <v>1200</v>
       </c>
-      <c r="I12" s="4">
-        <v>5</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
+        <v>5</v>
+      </c>
+      <c r="L12" s="4">
         <v>50</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="M12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>5002</v>
       </c>
@@ -1203,26 +1268,28 @@
       <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13">
         <v>160</v>
       </c>
-      <c r="G13" s="2">
+      <c r="I13" s="2">
         <v>110</v>
       </c>
-      <c r="H13" s="4">
+      <c r="J13" s="4">
         <v>1300</v>
       </c>
-      <c r="I13" s="4">
-        <v>5</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
+        <v>5</v>
+      </c>
+      <c r="L13" s="4">
         <v>55</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>5002</v>
       </c>
@@ -1238,26 +1305,28 @@
       <c r="E14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14">
         <v>180</v>
       </c>
-      <c r="G14" s="2">
+      <c r="I14" s="2">
         <v>120</v>
       </c>
-      <c r="H14" s="4">
+      <c r="J14" s="4">
         <v>1400</v>
       </c>
-      <c r="I14" s="4">
-        <v>5</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
+        <v>5</v>
+      </c>
+      <c r="L14" s="4">
         <v>60</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>5003</v>
       </c>
@@ -1273,26 +1342,32 @@
       <c r="E15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
+        <v>1002</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1004</v>
+      </c>
+      <c r="H15">
         <v>100</v>
       </c>
-      <c r="G15" s="2">
+      <c r="I15" s="2">
         <v>80</v>
       </c>
-      <c r="H15" s="4">
+      <c r="J15" s="4">
         <v>1000</v>
       </c>
-      <c r="I15" s="4">
-        <v>5</v>
-      </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
+        <v>5</v>
+      </c>
+      <c r="L15" s="4">
         <v>40</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>5003</v>
       </c>
@@ -1308,26 +1383,28 @@
       <c r="E16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16">
         <v>120</v>
       </c>
-      <c r="G16" s="2">
+      <c r="I16" s="2">
         <v>90</v>
       </c>
-      <c r="H16" s="4">
+      <c r="J16" s="4">
         <v>1100</v>
       </c>
-      <c r="I16" s="4">
-        <v>5</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
+        <v>5</v>
+      </c>
+      <c r="L16" s="4">
         <v>45</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>5003</v>
       </c>
@@ -1343,26 +1420,28 @@
       <c r="E17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17">
         <v>140</v>
       </c>
-      <c r="G17" s="2">
+      <c r="I17" s="2">
         <v>100</v>
       </c>
-      <c r="H17" s="4">
+      <c r="J17" s="4">
         <v>1200</v>
       </c>
-      <c r="I17" s="4">
-        <v>5</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
+        <v>5</v>
+      </c>
+      <c r="L17" s="4">
         <v>50</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>5003</v>
       </c>
@@ -1378,26 +1457,28 @@
       <c r="E18" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18">
         <v>160</v>
       </c>
-      <c r="G18" s="2">
+      <c r="I18" s="2">
         <v>110</v>
       </c>
-      <c r="H18" s="4">
+      <c r="J18" s="4">
         <v>1300</v>
       </c>
-      <c r="I18" s="4">
-        <v>5</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
+        <v>5</v>
+      </c>
+      <c r="L18" s="4">
         <v>55</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>5003</v>
       </c>
@@ -1413,26 +1494,28 @@
       <c r="E19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19">
         <v>180</v>
       </c>
-      <c r="G19" s="2">
+      <c r="I19" s="2">
         <v>120</v>
       </c>
-      <c r="H19" s="4">
+      <c r="J19" s="4">
         <v>1400</v>
       </c>
-      <c r="I19" s="4">
-        <v>5</v>
-      </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
+        <v>5</v>
+      </c>
+      <c r="L19" s="4">
         <v>60</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>5004</v>
       </c>
@@ -1448,26 +1531,32 @@
       <c r="E20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
+        <v>1003</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1004</v>
+      </c>
+      <c r="H20">
         <v>100</v>
       </c>
-      <c r="G20" s="2">
+      <c r="I20" s="2">
         <v>80</v>
       </c>
-      <c r="H20" s="4">
+      <c r="J20" s="4">
         <v>1000</v>
       </c>
-      <c r="I20" s="4">
-        <v>5</v>
-      </c>
-      <c r="J20" s="4">
+      <c r="K20" s="4">
+        <v>5</v>
+      </c>
+      <c r="L20" s="4">
         <v>40</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>5004</v>
       </c>
@@ -1483,26 +1572,28 @@
       <c r="E21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21">
         <v>120</v>
       </c>
-      <c r="G21" s="2">
+      <c r="I21" s="2">
         <v>90</v>
       </c>
-      <c r="H21" s="4">
+      <c r="J21" s="4">
         <v>1100</v>
       </c>
-      <c r="I21" s="4">
-        <v>5</v>
-      </c>
-      <c r="J21" s="4">
+      <c r="K21" s="4">
+        <v>5</v>
+      </c>
+      <c r="L21" s="4">
         <v>45</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>5004</v>
       </c>
@@ -1518,26 +1609,28 @@
       <c r="E22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22">
         <v>140</v>
       </c>
-      <c r="G22" s="2">
+      <c r="I22" s="2">
         <v>100</v>
       </c>
-      <c r="H22" s="4">
+      <c r="J22" s="4">
         <v>1200</v>
       </c>
-      <c r="I22" s="4">
-        <v>5</v>
-      </c>
-      <c r="J22" s="4">
+      <c r="K22" s="4">
+        <v>5</v>
+      </c>
+      <c r="L22" s="4">
         <v>50</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>5004</v>
       </c>
@@ -1553,26 +1646,28 @@
       <c r="E23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23">
         <v>160</v>
       </c>
-      <c r="G23" s="2">
+      <c r="I23" s="2">
         <v>110</v>
       </c>
-      <c r="H23" s="4">
+      <c r="J23" s="4">
         <v>1300</v>
       </c>
-      <c r="I23" s="4">
-        <v>5</v>
-      </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
+        <v>5</v>
+      </c>
+      <c r="L23" s="4">
         <v>55</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>5004</v>
       </c>
@@ -1588,26 +1683,28 @@
       <c r="E24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24">
         <v>180</v>
       </c>
-      <c r="G24" s="2">
+      <c r="I24" s="2">
         <v>120</v>
       </c>
-      <c r="H24" s="4">
+      <c r="J24" s="4">
         <v>1400</v>
       </c>
-      <c r="I24" s="4">
-        <v>5</v>
-      </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
+        <v>5</v>
+      </c>
+      <c r="L24" s="4">
         <v>60</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>5005</v>
       </c>
@@ -1623,26 +1720,32 @@
       <c r="E25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
+        <v>1002</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1004</v>
+      </c>
+      <c r="H25">
         <v>100</v>
       </c>
-      <c r="G25" s="2">
+      <c r="I25" s="2">
         <v>80</v>
       </c>
-      <c r="H25" s="4">
+      <c r="J25" s="4">
         <v>1000</v>
       </c>
-      <c r="I25" s="4">
-        <v>5</v>
-      </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
+        <v>5</v>
+      </c>
+      <c r="L25" s="4">
         <v>40</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>5005</v>
       </c>
@@ -1658,26 +1761,28 @@
       <c r="E26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26">
         <v>120</v>
       </c>
-      <c r="G26" s="2">
+      <c r="I26" s="2">
         <v>90</v>
       </c>
-      <c r="H26" s="4">
+      <c r="J26" s="4">
         <v>1100</v>
       </c>
-      <c r="I26" s="4">
-        <v>5</v>
-      </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
+        <v>5</v>
+      </c>
+      <c r="L26" s="4">
         <v>45</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="M26" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>5005</v>
       </c>
@@ -1693,26 +1798,28 @@
       <c r="E27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27">
         <v>140</v>
       </c>
-      <c r="G27" s="2">
+      <c r="I27" s="2">
         <v>100</v>
       </c>
-      <c r="H27" s="4">
+      <c r="J27" s="4">
         <v>1200</v>
       </c>
-      <c r="I27" s="4">
-        <v>5</v>
-      </c>
-      <c r="J27" s="4">
+      <c r="K27" s="4">
+        <v>5</v>
+      </c>
+      <c r="L27" s="4">
         <v>50</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>5005</v>
       </c>
@@ -1728,26 +1835,28 @@
       <c r="E28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28">
         <v>160</v>
       </c>
-      <c r="G28" s="2">
+      <c r="I28" s="2">
         <v>110</v>
       </c>
-      <c r="H28" s="4">
+      <c r="J28" s="4">
         <v>1300</v>
       </c>
-      <c r="I28" s="4">
-        <v>5</v>
-      </c>
-      <c r="J28" s="4">
+      <c r="K28" s="4">
+        <v>5</v>
+      </c>
+      <c r="L28" s="4">
         <v>55</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>5005</v>
       </c>
@@ -1763,22 +1872,24 @@
       <c r="E29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29">
         <v>180</v>
       </c>
-      <c r="G29" s="2">
+      <c r="I29" s="2">
         <v>120</v>
       </c>
-      <c r="H29" s="4">
+      <c r="J29" s="4">
         <v>1400</v>
       </c>
-      <c r="I29" s="4">
-        <v>5</v>
-      </c>
-      <c r="J29" s="4">
+      <c r="K29" s="4">
+        <v>5</v>
+      </c>
+      <c r="L29" s="4">
         <v>60</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>